<commit_message>
Fix SVM tables and plots
</commit_message>
<xml_diff>
--- a/Practica 2. SVM/resultados.xlsx
+++ b/Practica 2. SVM/resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Nextcloud\ETSINF\2019-20\APR\Practicas\Practica 2. SVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB86DE04-13F9-4B8B-84D8-C906CC3FF695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90D8AFD-8FD4-486D-A9B6-A22262BB1972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27300" windowHeight="15960" activeTab="2" xr2:uid="{D94C6A07-59AB-4FA3-8006-7B376ED6D8CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27300" windowHeight="15960" activeTab="1" xr2:uid="{D94C6A07-59AB-4FA3-8006-7B376ED6D8CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t>Separable</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Multiplicadores de Lagrange</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Vectores soporte</t>
@@ -88,21 +85,6 @@
     <t>Márgenes de tolerancia</t>
   </si>
   <si>
-    <t>(-0.61538, -0.92308)</t>
-  </si>
-  <si>
-    <t>(2, 3)</t>
-  </si>
-  <si>
-    <t>(3, 5)</t>
-  </si>
-  <si>
-    <t>(5, 4)</t>
-  </si>
-  <si>
-    <t>(-0.40000, -0.40000)</t>
-  </si>
-  <si>
     <t>Grado</t>
   </si>
   <si>
@@ -115,15 +97,6 @@
     <t>IC (95%)</t>
   </si>
   <si>
-    <t>(4. 2)</t>
-  </si>
-  <si>
-    <t>(-0.40000, -0.30000)</t>
-  </si>
-  <si>
-    <t>(-0.57139, -0.92308)</t>
-  </si>
-  <si>
     <t>(-1.00000, -1.49960)</t>
   </si>
 </sst>
@@ -131,9 +104,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
@@ -200,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -285,19 +257,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -319,17 +278,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -342,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -354,9 +302,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -372,6 +317,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,25 +344,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1815,469 +1754,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E25BF7D-9488-4919-8EF4-8E95BA198879}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="A1:E29"/>
+      <selection activeCell="D20" sqref="A1:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="7" max="10" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>3.3748999999999998</v>
+      </c>
+      <c r="C3" s="3">
+        <v>25.875</v>
+      </c>
+      <c r="D3" s="4">
+        <v>250.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
+      <c r="B4" s="3">
+        <v>5.7497999999999996</v>
+      </c>
+      <c r="C4" s="3">
+        <v>50.75</v>
+      </c>
+      <c r="D4" s="4">
+        <v>500.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
+      <c r="C5" s="3">
+        <v>100</v>
+      </c>
+      <c r="D5" s="4">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="3">
+        <v>-9.1247000000000007</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-76</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-751.62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="3">
+        <v>-10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-100</v>
+      </c>
+      <c r="D7" s="4">
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>7.9985999999999997</v>
+      </c>
+      <c r="C14" s="4">
+        <v>7.9987000000000004</v>
+      </c>
+      <c r="D14" s="4">
+        <v>7.9985999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1.1095999999999999</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.1096999999999999</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.1096999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="3">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="C17" s="3">
+        <v>-8.9999999999999998E-4</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="3">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0.65305999999999997</v>
-      </c>
-      <c r="D3" s="3">
-        <v>3.3748999999999998</v>
-      </c>
-      <c r="E3" s="4">
-        <v>250.87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.73472000000000004</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5.7497999999999996</v>
-      </c>
-      <c r="E4" s="4">
-        <v>500.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C6" s="3">
-        <v>-1</v>
-      </c>
-      <c r="D6" s="3">
-        <v>-9.1247000000000007</v>
-      </c>
-      <c r="E6" s="4">
-        <v>-751.62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="4">
-        <v>-0.1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>-0.38778000000000001</v>
-      </c>
-      <c r="D7" s="3">
-        <v>-10</v>
-      </c>
-      <c r="E7" s="4">
-        <v>-1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="4">
-        <v>-0.1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>-1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="4">
-        <v>-0.1</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="4">
-        <v>-0.1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1.4</v>
-      </c>
-      <c r="C20" s="4">
-        <v>5.0003000000000002</v>
+      <c r="C18" s="3">
+        <v>2.9986600000000001</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2.99865</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D19" s="3">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="3">
+        <v>0.49964999999999998</v>
+      </c>
+      <c r="C20" s="3">
+        <v>0.50112000000000001</v>
       </c>
       <c r="D20" s="3">
-        <v>7.9985999999999997</v>
-      </c>
-      <c r="E20" s="4">
-        <v>7.9985999999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="4">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4">
-        <v>1.9414</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1.1095999999999999</v>
-      </c>
-      <c r="E21" s="4">
-        <v>1.1096999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="C23" s="4">
-        <v>-2.5999999999999998E-4</v>
-      </c>
-      <c r="D23" s="3">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="C24" s="3">
-        <v>1.71418</v>
-      </c>
-      <c r="D24" s="3">
-        <v>3</v>
-      </c>
-      <c r="E24" s="3">
-        <v>2.99865</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0.85721999999999998</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0</v>
-      </c>
-      <c r="E25" s="3">
-        <v>8.9999999999999998E-4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="3">
-        <v>0</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0</v>
-      </c>
-      <c r="D26" s="3">
-        <v>0.49964999999999998</v>
-      </c>
-      <c r="E26" s="3">
         <v>0.50112999999999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="3">
-        <v>-0.3</v>
-      </c>
-      <c r="C27" s="3">
-        <v>1.1430400000000001</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="3">
-        <v>-0.8</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="3">
-        <v>-0.1</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A11:A18"/>
-    <mergeCell ref="A22:A29"/>
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2286,269 +2032,163 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7009C081-B551-4569-86C3-FF0758F1C55C}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="A1:E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
         <v>10</v>
       </c>
-      <c r="E2" s="6">
+      <c r="C2" s="5">
+        <v>100</v>
+      </c>
+      <c r="D2" s="5">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>0.1</v>
+        <v>0.87472000000000005</v>
       </c>
       <c r="C3" s="4">
-        <v>0.53846000000000005</v>
+        <v>0.87472000000000005</v>
       </c>
       <c r="D3" s="4">
         <v>0.87472000000000005</v>
       </c>
-      <c r="E3" s="4">
-        <v>0.87472000000000005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
       <c r="B4" s="4">
-        <v>0.1</v>
+        <v>0.74988999999999995</v>
       </c>
       <c r="C4" s="4">
-        <v>0.46154000000000001</v>
+        <v>0.74988999999999995</v>
       </c>
       <c r="D4" s="4">
         <v>0.74988999999999995</v>
       </c>
-      <c r="E4" s="4">
-        <v>0.74988999999999995</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
       <c r="B5" s="4">
-        <v>0.1</v>
+        <v>-1.6246100000000001</v>
       </c>
       <c r="C5" s="4">
-        <v>-1</v>
+        <v>-1.6246100000000001</v>
       </c>
       <c r="D5" s="4">
         <v>-1.6246100000000001</v>
       </c>
-      <c r="E5" s="4">
-        <v>-1.6246100000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="4">
-        <v>-0.1</v>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
-      <c r="B7" s="4">
-        <v>-0.1</v>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="4">
-        <v>-0.1</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
+        <v>7.9987000000000004</v>
+      </c>
+      <c r="C10" s="4">
+        <v>7.9987000000000004</v>
+      </c>
+      <c r="D10" s="4">
+        <v>7.9987000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="C15" s="4">
-        <v>5.3076999999999996</v>
-      </c>
-      <c r="D15" s="4">
-        <v>7.9987000000000004</v>
-      </c>
-      <c r="E15" s="4">
-        <v>7.9987000000000004</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="4">
-        <v>3.5354999999999999</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1.8028</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="B11" s="4">
         <v>1.1096999999999999</v>
       </c>
-      <c r="E16" s="4">
+      <c r="C11" s="4">
+        <v>1.1096999999999999</v>
+      </c>
+      <c r="D11" s="4">
         <v>1.1096999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2558,7 +2198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE046AE-22AA-4AC8-9CFA-1F8CAC7DB538}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
@@ -2570,147 +2210,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="A1" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>25</v>
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1.95</v>
       </c>
-      <c r="C3" s="9" t="str">
+      <c r="C3" s="8" t="str">
         <f>"±"&amp;TEXT(100*D3,"0.0000")&amp;"%"</f>
         <v>±0.1106%</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <f>1.96*SQRT((B3/100)*(1-(B3/100))/60000)</f>
         <v>1.1064239061047082E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>2.09</v>
       </c>
-      <c r="C4" s="9" t="str">
+      <c r="C4" s="8" t="str">
         <f>"±"&amp;TEXT(100*D4,"0.0000")&amp;"%"</f>
         <v>±0.1145%</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <f t="shared" ref="D4:D10" si="0">1.96*SQRT((B4/100)*(1-(B4/100))/60000)</f>
         <v>1.1446352454239153E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>2.63</v>
       </c>
-      <c r="C5" s="9" t="str">
+      <c r="C5" s="8" t="str">
         <f t="shared" ref="C5:C10" si="1">"±"&amp;TEXT(100*D5,"0.0000")&amp;"%"</f>
         <v>±0.1280%</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <f t="shared" si="0"/>
         <v>1.2804744153112418E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>3.35</v>
       </c>
-      <c r="C6" s="9" t="str">
+      <c r="C6" s="8" t="str">
         <f t="shared" si="1"/>
         <v>±0.1440%</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <f t="shared" si="0"/>
         <v>1.4398053363794243E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>4.12</v>
       </c>
-      <c r="C7" s="9" t="str">
+      <c r="C7" s="8" t="str">
         <f t="shared" si="1"/>
         <v>±0.1590%</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <f t="shared" si="0"/>
         <v>1.5903512950288688E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>5.27</v>
       </c>
-      <c r="C8" s="9" t="str">
+      <c r="C8" s="8" t="str">
         <f t="shared" si="1"/>
         <v>±0.1788%</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <f t="shared" si="0"/>
         <v>1.7878435927861996E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>6.36</v>
       </c>
-      <c r="C9" s="9" t="str">
+      <c r="C9" s="8" t="str">
         <f t="shared" si="1"/>
         <v>±0.1953%</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <f t="shared" si="0"/>
         <v>1.9527187955258687E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>7.42</v>
       </c>
-      <c r="C10" s="9" t="str">
+      <c r="C10" s="8" t="str">
         <f t="shared" si="1"/>
         <v>±0.2097%</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <f t="shared" si="0"/>
         <v>2.0972054953199031E-3</v>
       </c>

</xml_diff>

<commit_message>
Fix ICs and wording for Reports 1 & 2
</commit_message>
<xml_diff>
--- a/Practica 2. SVM/resultados.xlsx
+++ b/Practica 2. SVM/resultados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel\Nextcloud\ETSINF\2019-20\APR\Practicas\Practica 2. SVM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90D8AFD-8FD4-486D-A9B6-A22262BB1972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECE7041-CDA2-4041-9DA1-D81B9A72E2CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27300" windowHeight="15960" activeTab="1" xr2:uid="{D94C6A07-59AB-4FA3-8006-7B376ED6D8CD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27300" windowHeight="15960" activeTab="2" xr2:uid="{D94C6A07-59AB-4FA3-8006-7B376ED6D8CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -316,7 +316,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -481,9 +481,74 @@
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
-            <c:errValType val="percentage"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="5"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet2!$C$12:$C$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.27101740091735804</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.28037722928939862</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31365089462011742</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.3526788403065883</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.38955491845951579</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.43793045422304216</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.47831646601805372</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.51370833492946166</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet2!$C$12:$C$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.27101740091735804</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.28037722928939862</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31365089462011742</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.3526788403065883</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.38955491845951579</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.43793045422304216</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.47831646601805372</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.51370833492946166</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2034,8 +2099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7009C081-B551-4569-86C3-FF0758F1C55C}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,10 +2261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFE046AE-22AA-4AC8-9CFA-1F8CAC7DB538}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,11 +2301,11 @@
       </c>
       <c r="C3" s="8" t="str">
         <f>"±"&amp;TEXT(100*D3,"0.0000")&amp;"%"</f>
-        <v>±0.1106%</v>
+        <v>±0.2710%</v>
       </c>
       <c r="D3" s="9">
-        <f>1.96*SQRT((B3/100)*(1-(B3/100))/60000)</f>
-        <v>1.1064239061047082E-3</v>
+        <f>1.96*SQRT((B3/100)*(1-(B3/100))/10000)</f>
+        <v>2.7101740091735804E-3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2252,11 +2317,11 @@
       </c>
       <c r="C4" s="8" t="str">
         <f>"±"&amp;TEXT(100*D4,"0.0000")&amp;"%"</f>
-        <v>±0.1145%</v>
+        <v>±0.2804%</v>
       </c>
       <c r="D4" s="9">
-        <f t="shared" ref="D4:D10" si="0">1.96*SQRT((B4/100)*(1-(B4/100))/60000)</f>
-        <v>1.1446352454239153E-3</v>
+        <f t="shared" ref="D4:D10" si="0">1.96*SQRT((B4/100)*(1-(B4/100))/10000)</f>
+        <v>2.8037722928939864E-3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2268,11 +2333,11 @@
       </c>
       <c r="C5" s="8" t="str">
         <f t="shared" ref="C5:C10" si="1">"±"&amp;TEXT(100*D5,"0.0000")&amp;"%"</f>
-        <v>±0.1280%</v>
+        <v>±0.3137%</v>
       </c>
       <c r="D5" s="9">
         <f t="shared" si="0"/>
-        <v>1.2804744153112418E-3</v>
+        <v>3.1365089462011744E-3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2284,11 +2349,11 @@
       </c>
       <c r="C6" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>±0.1440%</v>
+        <v>±0.3527%</v>
       </c>
       <c r="D6" s="9">
         <f t="shared" si="0"/>
-        <v>1.4398053363794243E-3</v>
+        <v>3.5267884030658831E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2300,11 +2365,11 @@
       </c>
       <c r="C7" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>±0.1590%</v>
+        <v>±0.3896%</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="0"/>
-        <v>1.5903512950288688E-3</v>
+        <v>3.8955491845951581E-3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2316,11 +2381,11 @@
       </c>
       <c r="C8" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>±0.1788%</v>
+        <v>±0.4379%</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>1.7878435927861996E-3</v>
+        <v>4.3793045422304217E-3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2332,11 +2397,11 @@
       </c>
       <c r="C9" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>±0.1953%</v>
+        <v>±0.4783%</v>
       </c>
       <c r="D9" s="9">
         <f t="shared" si="0"/>
-        <v>1.9527187955258687E-3</v>
+        <v>4.7831646601805373E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2348,11 +2413,59 @@
       </c>
       <c r="C10" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>±0.2097%</v>
+        <v>±0.5137%</v>
       </c>
       <c r="D10" s="9">
         <f t="shared" si="0"/>
-        <v>2.0972054953199031E-3</v>
+        <v>5.1370833492946164E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f>100*D3</f>
+        <v>0.27101740091735804</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" ref="C13:C22" si="2">100*D4</f>
+        <v>0.28037722928939862</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>0.31365089462011742</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>0.3526788403065883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>0.38955491845951579</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>0.43793045422304216</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>0.47831646601805372</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>0.51370833492946166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>